<commit_message>
update project according to feedback
</commit_message>
<xml_diff>
--- a/src/test/resources/datadriven.xlsx
+++ b/src/test/resources/datadriven.xlsx
@@ -62,7 +62,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -97,12 +97,7 @@
       <color rgb="FF000C0B"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF6A8759"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -164,7 +159,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -248,10 +243,10 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.38"/>
   </cols>

</xml_diff>